<commit_message>
finished running the first cluster stuff with 100x100 worlds
</commit_message>
<xml_diff>
--- a/M0.4D0.0001E0.9A0.8_100x100_first_cluster.xlsx
+++ b/M0.4D0.0001E0.9A0.8_100x100_first_cluster.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B408"/>
+  <dimension ref="A1:B601"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4515,6 +4515,1936 @@
         <v>890001</v>
       </c>
     </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>00000851</t>
+        </is>
+      </c>
+      <c r="B409" t="n">
+        <v>95001</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>00000852</t>
+        </is>
+      </c>
+      <c r="B410" t="n">
+        <v>80001</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>00000849</t>
+        </is>
+      </c>
+      <c r="B411" t="n">
+        <v>1730001</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>00000846</t>
+        </is>
+      </c>
+      <c r="B412" t="n">
+        <v>3740001</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>00000854</t>
+        </is>
+      </c>
+      <c r="B413" t="n">
+        <v>260001</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>00000853</t>
+        </is>
+      </c>
+      <c r="B414" t="n">
+        <v>335001</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>00000858</t>
+        </is>
+      </c>
+      <c r="B415" t="n">
+        <v>95001</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>00000857</t>
+        </is>
+      </c>
+      <c r="B416" t="n">
+        <v>1220001</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>00000861</t>
+        </is>
+      </c>
+      <c r="B417" t="n">
+        <v>2735001</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>00000864</t>
+        </is>
+      </c>
+      <c r="B418" t="n">
+        <v>275001</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>00000855</t>
+        </is>
+      </c>
+      <c r="B419" t="n">
+        <v>5465001</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>00000866</t>
+        </is>
+      </c>
+      <c r="B420" t="n">
+        <v>815001</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>00000867</t>
+        </is>
+      </c>
+      <c r="B421" t="n">
+        <v>530001</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>00000859</t>
+        </is>
+      </c>
+      <c r="B422" t="n">
+        <v>6845001</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>00000869</t>
+        </is>
+      </c>
+      <c r="B423" t="n">
+        <v>170001</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>00000865</t>
+        </is>
+      </c>
+      <c r="B424" t="n">
+        <v>2975001</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>00000871</t>
+        </is>
+      </c>
+      <c r="B425" t="n">
+        <v>155001</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>00000872</t>
+        </is>
+      </c>
+      <c r="B426" t="n">
+        <v>155001</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>00000868</t>
+        </is>
+      </c>
+      <c r="B427" t="n">
+        <v>980001</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>00000870</t>
+        </is>
+      </c>
+      <c r="B428" t="n">
+        <v>680001</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>00000874</t>
+        </is>
+      </c>
+      <c r="B429" t="n">
+        <v>470001</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>00000876</t>
+        </is>
+      </c>
+      <c r="B430" t="n">
+        <v>995001</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>00000877</t>
+        </is>
+      </c>
+      <c r="B431" t="n">
+        <v>80001</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>00000875</t>
+        </is>
+      </c>
+      <c r="B432" t="n">
+        <v>1490001</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>00000878</t>
+        </is>
+      </c>
+      <c r="B433" t="n">
+        <v>200001</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>00000879</t>
+        </is>
+      </c>
+      <c r="B434" t="n">
+        <v>1190001</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>00000880</t>
+        </is>
+      </c>
+      <c r="B435" t="n">
+        <v>1145001</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>00000873</t>
+        </is>
+      </c>
+      <c r="B436" t="n">
+        <v>3530001</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>00000881</t>
+        </is>
+      </c>
+      <c r="B437" t="n">
+        <v>590001</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>00000882</t>
+        </is>
+      </c>
+      <c r="B438" t="n">
+        <v>950001</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>00000885</t>
+        </is>
+      </c>
+      <c r="B439" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>00000884</t>
+        </is>
+      </c>
+      <c r="B440" t="n">
+        <v>515001</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>00000883</t>
+        </is>
+      </c>
+      <c r="B441" t="n">
+        <v>800001</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>00000888</t>
+        </is>
+      </c>
+      <c r="B442" t="n">
+        <v>485001</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>00000889</t>
+        </is>
+      </c>
+      <c r="B443" t="n">
+        <v>560001</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>00000886</t>
+        </is>
+      </c>
+      <c r="B444" t="n">
+        <v>2030001</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>00000887</t>
+        </is>
+      </c>
+      <c r="B445" t="n">
+        <v>2300001</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>00000892</t>
+        </is>
+      </c>
+      <c r="B446" t="n">
+        <v>590001</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>00000893</t>
+        </is>
+      </c>
+      <c r="B447" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>00000890</t>
+        </is>
+      </c>
+      <c r="B448" t="n">
+        <v>1955001</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>00000891</t>
+        </is>
+      </c>
+      <c r="B449" t="n">
+        <v>1400001</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>00000895</t>
+        </is>
+      </c>
+      <c r="B450" t="n">
+        <v>290001</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>00000896</t>
+        </is>
+      </c>
+      <c r="B451" t="n">
+        <v>170001</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>00000898</t>
+        </is>
+      </c>
+      <c r="B452" t="n">
+        <v>140001</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>00000897</t>
+        </is>
+      </c>
+      <c r="B453" t="n">
+        <v>185001</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>00000900</t>
+        </is>
+      </c>
+      <c r="B454" t="n">
+        <v>80001</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>00000899</t>
+        </is>
+      </c>
+      <c r="B455" t="n">
+        <v>185001</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>00000894</t>
+        </is>
+      </c>
+      <c r="B456" t="n">
+        <v>890001</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>00000901</t>
+        </is>
+      </c>
+      <c r="B457" t="n">
+        <v>275001</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>00000902</t>
+        </is>
+      </c>
+      <c r="B458" t="n">
+        <v>245001</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>00000903</t>
+        </is>
+      </c>
+      <c r="B459" t="n">
+        <v>380001</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>00000904</t>
+        </is>
+      </c>
+      <c r="B460" t="n">
+        <v>320001</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>00000906</t>
+        </is>
+      </c>
+      <c r="B461" t="n">
+        <v>95001</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>00000907</t>
+        </is>
+      </c>
+      <c r="B462" t="n">
+        <v>65001</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>00000908</t>
+        </is>
+      </c>
+      <c r="B463" t="n">
+        <v>155001</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>00000910</t>
+        </is>
+      </c>
+      <c r="B464" t="n">
+        <v>290001</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>00000911</t>
+        </is>
+      </c>
+      <c r="B465" t="n">
+        <v>80001</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>00000912</t>
+        </is>
+      </c>
+      <c r="B466" t="n">
+        <v>170001</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>00000913</t>
+        </is>
+      </c>
+      <c r="B467" t="n">
+        <v>230001</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>00000914</t>
+        </is>
+      </c>
+      <c r="B468" t="n">
+        <v>275001</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>00000909</t>
+        </is>
+      </c>
+      <c r="B469" t="n">
+        <v>1295001</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>00000915</t>
+        </is>
+      </c>
+      <c r="B470" t="n">
+        <v>125001</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>00000917</t>
+        </is>
+      </c>
+      <c r="B471" t="n">
+        <v>470001</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>00000918</t>
+        </is>
+      </c>
+      <c r="B472" t="n">
+        <v>1010001</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>00000919</t>
+        </is>
+      </c>
+      <c r="B473" t="n">
+        <v>290001</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>00000920</t>
+        </is>
+      </c>
+      <c r="B474" t="n">
+        <v>155001</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>00000921</t>
+        </is>
+      </c>
+      <c r="B475" t="n">
+        <v>770001</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>00000922</t>
+        </is>
+      </c>
+      <c r="B476" t="n">
+        <v>575001</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>00000916</t>
+        </is>
+      </c>
+      <c r="B477" t="n">
+        <v>3620001</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>00000923</t>
+        </is>
+      </c>
+      <c r="B478" t="n">
+        <v>200001</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>00000925</t>
+        </is>
+      </c>
+      <c r="B479" t="n">
+        <v>65001</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>00000924</t>
+        </is>
+      </c>
+      <c r="B480" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>00000927</t>
+        </is>
+      </c>
+      <c r="B481" t="n">
+        <v>170001</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>00000928</t>
+        </is>
+      </c>
+      <c r="B482" t="n">
+        <v>425001</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>00000926</t>
+        </is>
+      </c>
+      <c r="B483" t="n">
+        <v>635001</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>00000930</t>
+        </is>
+      </c>
+      <c r="B484" t="n">
+        <v>65001</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>00000931</t>
+        </is>
+      </c>
+      <c r="B485" t="n">
+        <v>185001</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>00000932</t>
+        </is>
+      </c>
+      <c r="B486" t="n">
+        <v>320001</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>00000933</t>
+        </is>
+      </c>
+      <c r="B487" t="n">
+        <v>185001</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>00000934</t>
+        </is>
+      </c>
+      <c r="B488" t="n">
+        <v>125001</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>00000905</t>
+        </is>
+      </c>
+      <c r="B489" t="n">
+        <v>7700001</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>00000936</t>
+        </is>
+      </c>
+      <c r="B490" t="n">
+        <v>185001</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>00000935</t>
+        </is>
+      </c>
+      <c r="B491" t="n">
+        <v>890001</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>00000938</t>
+        </is>
+      </c>
+      <c r="B492" t="n">
+        <v>725001</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>00000939</t>
+        </is>
+      </c>
+      <c r="B493" t="n">
+        <v>410001</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>00000940</t>
+        </is>
+      </c>
+      <c r="B494" t="n">
+        <v>140001</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>00000929</t>
+        </is>
+      </c>
+      <c r="B495" t="n">
+        <v>3680001</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>00000941</t>
+        </is>
+      </c>
+      <c r="B496" t="n">
+        <v>905001</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>00000943</t>
+        </is>
+      </c>
+      <c r="B497" t="n">
+        <v>185001</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>00000937</t>
+        </is>
+      </c>
+      <c r="B498" t="n">
+        <v>3215001</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>00000945</t>
+        </is>
+      </c>
+      <c r="B499" t="n">
+        <v>95001</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>00000946</t>
+        </is>
+      </c>
+      <c r="B500" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>00000947</t>
+        </is>
+      </c>
+      <c r="B501" t="n">
+        <v>170001</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>00000948</t>
+        </is>
+      </c>
+      <c r="B502" t="n">
+        <v>365001</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>00000949</t>
+        </is>
+      </c>
+      <c r="B503" t="n">
+        <v>155001</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>00000950</t>
+        </is>
+      </c>
+      <c r="B504" t="n">
+        <v>200001</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>00000951</t>
+        </is>
+      </c>
+      <c r="B505" t="n">
+        <v>80001</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>00000942</t>
+        </is>
+      </c>
+      <c r="B506" t="n">
+        <v>2840001</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>00000944</t>
+        </is>
+      </c>
+      <c r="B507" t="n">
+        <v>2495001</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>00000952</t>
+        </is>
+      </c>
+      <c r="B508" t="n">
+        <v>905001</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>00000954</t>
+        </is>
+      </c>
+      <c r="B509" t="n">
+        <v>350001</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>00000955</t>
+        </is>
+      </c>
+      <c r="B510" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>00000956</t>
+        </is>
+      </c>
+      <c r="B511" t="n">
+        <v>215001</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>00000958</t>
+        </is>
+      </c>
+      <c r="B512" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>00000953</t>
+        </is>
+      </c>
+      <c r="B513" t="n">
+        <v>950001</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>00000957</t>
+        </is>
+      </c>
+      <c r="B514" t="n">
+        <v>455001</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>00000960</t>
+        </is>
+      </c>
+      <c r="B515" t="n">
+        <v>245001</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>00000962</t>
+        </is>
+      </c>
+      <c r="B516" t="n">
+        <v>65001</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>00000961</t>
+        </is>
+      </c>
+      <c r="B517" t="n">
+        <v>1385001</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>00000963</t>
+        </is>
+      </c>
+      <c r="B518" t="n">
+        <v>1325001</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>00000965</t>
+        </is>
+      </c>
+      <c r="B519" t="n">
+        <v>185001</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>00000964</t>
+        </is>
+      </c>
+      <c r="B520" t="n">
+        <v>515001</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>00000966</t>
+        </is>
+      </c>
+      <c r="B521" t="n">
+        <v>380001</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>00000967</t>
+        </is>
+      </c>
+      <c r="B522" t="n">
+        <v>335001</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>00000968</t>
+        </is>
+      </c>
+      <c r="B523" t="n">
+        <v>80001</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>00000969</t>
+        </is>
+      </c>
+      <c r="B524" t="n">
+        <v>185001</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>00000971</t>
+        </is>
+      </c>
+      <c r="B525" t="n">
+        <v>350001</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>00000970</t>
+        </is>
+      </c>
+      <c r="B526" t="n">
+        <v>1475001</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>00000973</t>
+        </is>
+      </c>
+      <c r="B527" t="n">
+        <v>125001</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>00000972</t>
+        </is>
+      </c>
+      <c r="B528" t="n">
+        <v>1385001</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>00000975</t>
+        </is>
+      </c>
+      <c r="B529" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>00000976</t>
+        </is>
+      </c>
+      <c r="B530" t="n">
+        <v>245001</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>00000977</t>
+        </is>
+      </c>
+      <c r="B531" t="n">
+        <v>65001</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>00000978</t>
+        </is>
+      </c>
+      <c r="B532" t="n">
+        <v>560001</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>00000979</t>
+        </is>
+      </c>
+      <c r="B533" t="n">
+        <v>1655001</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>00000980</t>
+        </is>
+      </c>
+      <c r="B534" t="n">
+        <v>125001</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>00000981</t>
+        </is>
+      </c>
+      <c r="B535" t="n">
+        <v>245001</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>00000974</t>
+        </is>
+      </c>
+      <c r="B536" t="n">
+        <v>4505001</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>00000983</t>
+        </is>
+      </c>
+      <c r="B537" t="n">
+        <v>425001</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>00000984</t>
+        </is>
+      </c>
+      <c r="B538" t="n">
+        <v>695001</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>00000985</t>
+        </is>
+      </c>
+      <c r="B539" t="n">
+        <v>410001</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>00000986</t>
+        </is>
+      </c>
+      <c r="B540" t="n">
+        <v>170001</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>00000982</t>
+        </is>
+      </c>
+      <c r="B541" t="n">
+        <v>3020001</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>00000988</t>
+        </is>
+      </c>
+      <c r="B542" t="n">
+        <v>95001</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>00000987</t>
+        </is>
+      </c>
+      <c r="B543" t="n">
+        <v>290001</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>00000989</t>
+        </is>
+      </c>
+      <c r="B544" t="n">
+        <v>140001</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>00000991</t>
+        </is>
+      </c>
+      <c r="B545" t="n">
+        <v>95001</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>00000992</t>
+        </is>
+      </c>
+      <c r="B546" t="n">
+        <v>95001</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>00000993</t>
+        </is>
+      </c>
+      <c r="B547" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>00000959</t>
+        </is>
+      </c>
+      <c r="B548" t="n">
+        <v>11135001</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>00000994</t>
+        </is>
+      </c>
+      <c r="B549" t="n">
+        <v>515001</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>00000990</t>
+        </is>
+      </c>
+      <c r="B550" t="n">
+        <v>1370001</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>00000997</t>
+        </is>
+      </c>
+      <c r="B551" t="n">
+        <v>185001</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>00000998</t>
+        </is>
+      </c>
+      <c r="B552" t="n">
+        <v>170001</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>00000999</t>
+        </is>
+      </c>
+      <c r="B553" t="n">
+        <v>125001</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>00000996</t>
+        </is>
+      </c>
+      <c r="B554" t="n">
+        <v>1355001</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>00001001</t>
+        </is>
+      </c>
+      <c r="B555" t="n">
+        <v>230001</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>00001000</t>
+        </is>
+      </c>
+      <c r="B556" t="n">
+        <v>545001</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>00001003</t>
+        </is>
+      </c>
+      <c r="B557" t="n">
+        <v>65001</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>00001002</t>
+        </is>
+      </c>
+      <c r="B558" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>00001005</t>
+        </is>
+      </c>
+      <c r="B559" t="n">
+        <v>170001</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>00001006</t>
+        </is>
+      </c>
+      <c r="B560" t="n">
+        <v>755001</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>00000995</t>
+        </is>
+      </c>
+      <c r="B561" t="n">
+        <v>3170001</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>00001007</t>
+        </is>
+      </c>
+      <c r="B562" t="n">
+        <v>545001</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>00001008</t>
+        </is>
+      </c>
+      <c r="B563" t="n">
+        <v>380001</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>00001009</t>
+        </is>
+      </c>
+      <c r="B564" t="n">
+        <v>230001</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>00001010</t>
+        </is>
+      </c>
+      <c r="B565" t="n">
+        <v>620001</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>00001011</t>
+        </is>
+      </c>
+      <c r="B566" t="n">
+        <v>1400001</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>00001004</t>
+        </is>
+      </c>
+      <c r="B567" t="n">
+        <v>4520001</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>00001012</t>
+        </is>
+      </c>
+      <c r="B568" t="n">
+        <v>770001</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>00001013</t>
+        </is>
+      </c>
+      <c r="B569" t="n">
+        <v>65001</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>00001014</t>
+        </is>
+      </c>
+      <c r="B570" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>00001016</t>
+        </is>
+      </c>
+      <c r="B571" t="n">
+        <v>200001</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>00001017</t>
+        </is>
+      </c>
+      <c r="B572" t="n">
+        <v>230001</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>00001018</t>
+        </is>
+      </c>
+      <c r="B573" t="n">
+        <v>1070001</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>00001015</t>
+        </is>
+      </c>
+      <c r="B574" t="n">
+        <v>1760001</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>00001020</t>
+        </is>
+      </c>
+      <c r="B575" t="n">
+        <v>365001</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>00001019</t>
+        </is>
+      </c>
+      <c r="B576" t="n">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>00001021</t>
+        </is>
+      </c>
+      <c r="B577" t="n">
+        <v>1115001</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>00001023</t>
+        </is>
+      </c>
+      <c r="B578" t="n">
+        <v>80001</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>00001024</t>
+        </is>
+      </c>
+      <c r="B579" t="n">
+        <v>2885001</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>00001025</t>
+        </is>
+      </c>
+      <c r="B580" t="n">
+        <v>95001</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>00001026</t>
+        </is>
+      </c>
+      <c r="B581" t="n">
+        <v>245001</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>00001027</t>
+        </is>
+      </c>
+      <c r="B582" t="n">
+        <v>740001</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>00001028</t>
+        </is>
+      </c>
+      <c r="B583" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>00001029</t>
+        </is>
+      </c>
+      <c r="B584" t="n">
+        <v>515001</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>00001022</t>
+        </is>
+      </c>
+      <c r="B585" t="n">
+        <v>7835001</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>00001030</t>
+        </is>
+      </c>
+      <c r="B586" t="n">
+        <v>3275001</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>00001031</t>
+        </is>
+      </c>
+      <c r="B587" t="n">
+        <v>1520001</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>00001033</t>
+        </is>
+      </c>
+      <c r="B588" t="n">
+        <v>155001</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>00001032</t>
+        </is>
+      </c>
+      <c r="B589" t="n">
+        <v>635001</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>00001035</t>
+        </is>
+      </c>
+      <c r="B590" t="n">
+        <v>185001</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>00001036</t>
+        </is>
+      </c>
+      <c r="B591" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>00001037</t>
+        </is>
+      </c>
+      <c r="B592" t="n">
+        <v>230001</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>00001034</t>
+        </is>
+      </c>
+      <c r="B593" t="n">
+        <v>905001</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>00001038</t>
+        </is>
+      </c>
+      <c r="B594" t="n">
+        <v>500001</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>00001039</t>
+        </is>
+      </c>
+      <c r="B595" t="n">
+        <v>125001</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>00001040</t>
+        </is>
+      </c>
+      <c r="B596" t="n">
+        <v>110001</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>00001041</t>
+        </is>
+      </c>
+      <c r="B597" t="n">
+        <v>770001</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>00001042</t>
+        </is>
+      </c>
+      <c r="B598" t="n">
+        <v>1445001</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>00001044</t>
+        </is>
+      </c>
+      <c r="B599" t="n">
+        <v>80001</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>00001045</t>
+        </is>
+      </c>
+      <c r="B600" t="n">
+        <v>455001</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>00001046</t>
+        </is>
+      </c>
+      <c r="B601" t="n">
+        <v>110001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>